<commit_message>
Author            : Prateek Kapoor File Modified     : DbSchema NSKFDC-App.xlsx Description       : Added table for reports upload
</commit_message>
<xml_diff>
--- a/Database/DbSchema/DbSchema NSKFDC-App.xlsx
+++ b/Database/DbSchema/DbSchema NSKFDC-App.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashmi kapoor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashmi kapoor\Desktop\NSKFDC APP\trunk\Database\DbSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{83029DAC-6AC8-4A49-A97B-F8F3B077D507}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{58F5ED76-ED37-41EF-9259-3974ECF2BE20}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{277FC6CD-DE18-4ECF-921F-C7FF6CEEBD2E}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>Candidate</t>
   </si>
@@ -211,9 +211,6 @@
     <t>wardNumber</t>
   </si>
   <si>
-    <t>scgjBatchNumber</t>
-  </si>
-  <si>
     <t>CentreDetails</t>
   </si>
   <si>
@@ -260,6 +257,45 @@
   </si>
   <si>
     <t xml:space="preserve"> trainingPartnerEmail - unique</t>
+  </si>
+  <si>
+    <t>reportId (Auto Increment)</t>
+  </si>
+  <si>
+    <t>reportType</t>
+  </si>
+  <si>
+    <t>reportPath</t>
+  </si>
+  <si>
+    <t>batchId - FK</t>
+  </si>
+  <si>
+    <t>trainingPartnerEmail - FK</t>
+  </si>
+  <si>
+    <t>occupationCertificate  - Flag</t>
+  </si>
+  <si>
+    <t>attendanceSheet - Flag</t>
+  </si>
+  <si>
+    <t>nskfdcSheet - Flag</t>
+  </si>
+  <si>
+    <t>finalBatchReport - Flag</t>
+  </si>
+  <si>
+    <t>scgjBatchNumber - unique</t>
+  </si>
+  <si>
+    <t>sdmsSheet - Flag</t>
+  </si>
+  <si>
+    <t>UploadReports</t>
+  </si>
+  <si>
+    <t>selectionCommittee - Flag</t>
   </si>
 </sst>
 </file>
@@ -696,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334A76D3-B951-47A5-9EF4-C93B2ED3C2EE}">
-  <dimension ref="A5:H30"/>
+  <dimension ref="A3:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,9 +752,10 @@
     <col min="11" max="11" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
@@ -735,7 +772,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>3</v>
@@ -751,7 +788,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>1</v>
@@ -767,7 +804,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>2</v>
@@ -783,7 +820,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
@@ -816,6 +853,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -824,10 +864,13 @@
         <v>31</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
@@ -838,6 +881,9 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
@@ -847,6 +893,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
@@ -855,10 +904,13 @@
         <v>35</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
@@ -867,10 +919,13 @@
         <v>36</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
@@ -879,10 +934,13 @@
         <v>37</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
@@ -891,10 +949,13 @@
         <v>38</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="C19" s="5" t="s">
         <v>7</v>
       </c>
@@ -903,10 +964,13 @@
         <v>48</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
@@ -918,16 +982,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C22" s="5" t="s">
         <v>10</v>
       </c>
@@ -936,19 +1006,22 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="C23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
         <v>19</v>
       </c>
@@ -957,10 +1030,10 @@
         <v>39</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="5" t="s">
         <v>20</v>
       </c>
@@ -969,19 +1042,19 @@
         <v>40</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="7"/>
       <c r="G26" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
         <v>22</v>
       </c>
@@ -990,19 +1063,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C30" s="5" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
author: Samridhi tables altered: Candidate Schema description: The candidate id is not a relevant field for batch id. The candidate schema should have a batch id field.
</commit_message>
<xml_diff>
--- a/Database/DbSchema/DbSchema NSKFDC-App.xlsx
+++ b/Database/DbSchema/DbSchema NSKFDC-App.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashmi kapoor\Desktop\NSKFDC APP\trunk\Database\DbSchema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samridhi Srivastava\Desktop\NSKFDC\trunk\Database\DbSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{58F5ED76-ED37-41EF-9259-3974ECF2BE20}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{277FC6CD-DE18-4ECF-921F-C7FF6CEEBD2E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>prateek kapoor</author>
   </authors>
   <commentList>
-    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{96F0544D-66D9-4120-B5E9-FC5396E202D0}">
+    <comment ref="E24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>Candidate</t>
   </si>
@@ -136,9 +138,6 @@
     <t>assessmentResult</t>
   </si>
   <si>
-    <t>medicalExamStatus</t>
-  </si>
-  <si>
     <t>BankDetails</t>
   </si>
   <si>
@@ -181,9 +180,6 @@
     <t>nsdcRegNumber - FK</t>
   </si>
   <si>
-    <t>candidateId - FK</t>
-  </si>
-  <si>
     <t>TrainingPartnerDetails</t>
   </si>
   <si>
@@ -211,6 +207,9 @@
     <t>wardNumber</t>
   </si>
   <si>
+    <t>scgjBatchNumber</t>
+  </si>
+  <si>
     <t>CentreDetails</t>
   </si>
   <si>
@@ -259,49 +258,19 @@
     <t xml:space="preserve"> trainingPartnerEmail - unique</t>
   </si>
   <si>
-    <t>reportId (Auto Increment)</t>
-  </si>
-  <si>
-    <t>reportType</t>
-  </si>
-  <si>
-    <t>reportPath</t>
-  </si>
-  <si>
-    <t>batchId - FK</t>
-  </si>
-  <si>
-    <t>trainingPartnerEmail - FK</t>
-  </si>
-  <si>
-    <t>occupationCertificate  - Flag</t>
-  </si>
-  <si>
-    <t>attendanceSheet - Flag</t>
-  </si>
-  <si>
-    <t>nskfdcSheet - Flag</t>
-  </si>
-  <si>
-    <t>finalBatchReport - Flag</t>
-  </si>
-  <si>
-    <t>scgjBatchNumber - unique</t>
-  </si>
-  <si>
-    <t>sdmsSheet - Flag</t>
-  </si>
-  <si>
-    <t>UploadReports</t>
-  </si>
-  <si>
-    <t>selectionCommittee - Flag</t>
+    <t>batchId-FK</t>
+  </si>
+  <si>
+    <t>medicalExamConducted(Flag)</t>
+  </si>
+  <si>
+    <t>medicalExamDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -373,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -396,11 +365,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -418,12 +398,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -731,11 +741,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334A76D3-B951-47A5-9EF4-C93B2ED3C2EE}">
-  <dimension ref="A3:H30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,10 +762,9 @@
     <col min="11" max="11" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
@@ -763,75 +772,75 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -840,7 +849,7 @@
       </c>
       <c r="D10" s="7"/>
       <c r="G10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -849,237 +858,206 @@
       </c>
       <c r="D11" s="7"/>
       <c r="G11" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>72</v>
-      </c>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="5" t="s">
-        <v>37</v>
+      <c r="E17" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>73</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>74</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>76</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>78</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>69</v>
-      </c>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="5" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="10" t="s">
-        <v>39</v>
+      <c r="E24" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="7"/>
       <c r="G26" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="7"/>
       <c r="G27" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="5" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="13" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Author           : Prateek Kapoor File Modified    : DbSchema NSKFDC-App.xlsx Description      : Added table for upload documents
</commit_message>
<xml_diff>
--- a/Database/DbSchema/DbSchema NSKFDC-App.xlsx
+++ b/Database/DbSchema/DbSchema NSKFDC-App.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samridhi Srivastava\Desktop\NSKFDC\trunk\Database\DbSchema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashmi kapoor\Desktop\NSKFDC APP\trunk\Database\DbSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{797E7DF5-B7E8-4E90-B48A-73D5B91CE7A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>prateek kapoor</author>
   </authors>
   <commentList>
-    <comment ref="E24" authorId="0" shapeId="0">
+    <comment ref="E24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t>Candidate</t>
   </si>
@@ -265,13 +266,49 @@
   </si>
   <si>
     <t>medicalExamDate</t>
+  </si>
+  <si>
+    <t>UploadedDocuments</t>
+  </si>
+  <si>
+    <t>id(Auto Increment) - PK</t>
+  </si>
+  <si>
+    <t>finalBatchReport - Flag</t>
+  </si>
+  <si>
+    <t>occupationCertificate - Flag</t>
+  </si>
+  <si>
+    <t>minuteOfSelectionCommittee - Flag</t>
+  </si>
+  <si>
+    <t>dataSheetForSDDMS - Flag</t>
+  </si>
+  <si>
+    <t>dataSheetForNSKFC - Flag</t>
+  </si>
+  <si>
+    <t>attendanceSheet - Flag</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>dateUploaded (date)</t>
+  </si>
+  <si>
+    <t>batchId - FK</t>
+  </si>
+  <si>
+    <t>trainingPartnerId - FK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +357,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -380,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -398,8 +442,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +474,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -741,17 +786,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
@@ -862,6 +907,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -874,6 +922,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>69</v>
+      </c>
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
@@ -884,6 +935,9 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
@@ -893,6 +947,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
@@ -905,6 +962,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
@@ -916,19 +976,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>67</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
@@ -940,7 +1006,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="C19" s="5" t="s">
         <v>7</v>
       </c>
@@ -952,7 +1021,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
@@ -964,7 +1036,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
@@ -973,7 +1048,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="C22" s="5" t="s">
         <v>10</v>
       </c>
@@ -982,7 +1060,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="C23" s="5" t="s">
         <v>11</v>
       </c>
@@ -994,7 +1075,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
         <v>19</v>
       </c>
@@ -1006,7 +1087,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="5" t="s">
         <v>20</v>
       </c>
@@ -1018,7 +1099,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1108,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
         <v>22</v>
       </c>
@@ -1036,26 +1117,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C30" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="13" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="14" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Author        : Sarthak (Reviewed by Prateek) File Modified : DbSchema NSKFDC-App.xlsx Description   : Necessary changes done for TpEmailId (NsdcRegNum replaced by TpEmailId)
</commit_message>
<xml_diff>
--- a/Database/DbSchema/DbSchema NSKFDC-App.xlsx
+++ b/Database/DbSchema/DbSchema NSKFDC-App.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>Candidate</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>municipality</t>
-  </si>
-  <si>
-    <t>nsdcRegNumber - FK</t>
   </si>
   <si>
     <t>TrainingPartnerDetails</t>
@@ -806,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,7 +823,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
@@ -838,12 +835,12 @@
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -854,12 +851,12 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>1</v>
@@ -870,12 +867,12 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>2</v>
@@ -886,12 +883,12 @@
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>4</v>
@@ -902,7 +899,7 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -920,12 +917,12 @@
       </c>
       <c r="D8" s="7"/>
       <c r="G8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>13</v>
@@ -935,12 +932,12 @@
         <v>30</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>14</v>
@@ -953,7 +950,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>15</v>
@@ -965,7 +962,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>16</v>
@@ -975,44 +972,44 @@
         <v>34</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>6</v>
@@ -1022,12 +1019,12 @@
         <v>36</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>7</v>
@@ -1037,108 +1034,108 @@
         <v>37</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="10" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="7"/>
       <c r="G23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>22</v>
@@ -1150,7 +1147,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>23</v>
@@ -1165,13 +1162,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Author : Mannu Kumari Files Added : Updated Final Master Sheet.xlsx and Updated DbSchema NSKFDC-App.xlsx
</commit_message>
<xml_diff>
--- a/Database/DbSchema/DbSchema NSKFDC-App.xlsx
+++ b/Database/DbSchema/DbSchema NSKFDC-App.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NSKFDC-App.git\trunk\Database\DbSchema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mannu Kumari\Desktop\Assessment\trunk\Database\DbSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7ABB6E11-1147-4993-A6CB-5C67E4A0AB86}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>Candidate</t>
   </si>
@@ -280,12 +279,15 @@
   </si>
   <si>
     <t>trainingPartnerEmail - FK</t>
+  </si>
+  <si>
+    <t>age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,7 +441,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -751,11 +753,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +980,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="5" t="s">
@@ -993,7 +995,7 @@
         <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="5" t="s">
@@ -1008,7 +1010,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="5" t="s">
@@ -1020,7 +1022,7 @@
         <v>78</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="5" t="s">
@@ -1032,7 +1034,7 @@
         <v>79</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="5" t="s">
@@ -1047,7 +1049,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="10" t="s">
@@ -1062,7 +1064,7 @@
         <v>81</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="7"/>
       <c r="G22" s="5" t="s">
@@ -1074,7 +1076,7 @@
         <v>74</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="7"/>
       <c r="G23" s="5" t="s">
@@ -1086,7 +1088,7 @@
         <v>75</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="7"/>
       <c r="G24" s="10" t="s">
@@ -1098,24 +1100,29 @@
         <v>83</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="14" t="s">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="14" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Author : Mannu Kumari Files Updated : DbSchema NSKFDC-App.xlsx Description : GenerateReports Table added in the DBSchema.
</commit_message>
<xml_diff>
--- a/Database/DbSchema/DbSchema NSKFDC-App.xlsx
+++ b/Database/DbSchema/DbSchema NSKFDC-App.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>Candidate</t>
   </si>
@@ -282,6 +282,45 @@
   </si>
   <si>
     <t>age</t>
+  </si>
+  <si>
+    <t>GenerateReports</t>
+  </si>
+  <si>
+    <t>NSKFDCSheet - Flag</t>
+  </si>
+  <si>
+    <t>occupationReport - Flag</t>
+  </si>
+  <si>
+    <t>SDMSSheet - Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selectionCommittee - Flag </t>
+  </si>
+  <si>
+    <t>batchReport - Flag</t>
+  </si>
+  <si>
+    <t>ORGeneratedOn</t>
+  </si>
+  <si>
+    <t>ASGeneratedOn</t>
+  </si>
+  <si>
+    <t>NSKFDCGeneratedOn</t>
+  </si>
+  <si>
+    <t>SDMSGeneratedOn</t>
+  </si>
+  <si>
+    <t>SCGeneratedOn</t>
+  </si>
+  <si>
+    <t>BRGeneratedOn</t>
+  </si>
+  <si>
+    <t>generateReportsId (Auto Increment )- PK</t>
   </si>
 </sst>
 </file>
@@ -391,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -412,6 +451,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H29"/>
+  <dimension ref="A2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,12 +810,12 @@
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.42578125" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>57</v>
       </c>
@@ -790,8 +831,11 @@
       <c r="G2" s="9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -806,8 +850,11 @@
       <c r="G3" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -822,8 +869,11 @@
       <c r="G4" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -838,8 +888,11 @@
       <c r="G5" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>60</v>
       </c>
@@ -854,8 +907,11 @@
       <c r="G6" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -863,8 +919,14 @@
       <c r="G7" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
@@ -872,8 +934,11 @@
       <c r="G8" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>66</v>
       </c>
@@ -887,8 +952,11 @@
       <c r="G9" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>67</v>
       </c>
@@ -900,8 +968,11 @@
         <v>31</v>
       </c>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>68</v>
       </c>
@@ -912,8 +983,14 @@
       <c r="E11" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>69</v>
       </c>
@@ -927,8 +1004,11 @@
       <c r="G12" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
@@ -944,8 +1024,11 @@
       <c r="G13" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
@@ -959,8 +1042,11 @@
       <c r="G14" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
@@ -974,8 +1060,11 @@
       <c r="G15" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>73</v>
       </c>
@@ -989,8 +1078,11 @@
       <c r="G16" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
@@ -1004,8 +1096,11 @@
       <c r="G17" s="10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>77</v>
       </c>
@@ -1017,7 +1112,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>78</v>
       </c>
@@ -1029,7 +1124,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -1044,7 +1139,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>80</v>
       </c>
@@ -1059,7 +1154,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>81</v>
       </c>
@@ -1071,7 +1166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>74</v>
       </c>
@@ -1083,7 +1178,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>75</v>
       </c>
@@ -1095,7 +1190,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>83</v>
       </c>
@@ -1104,24 +1199,24 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" s="14" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Author   : Priyanka Chaudhary Description : Database Schema Updated, autoincremented batchId & generateReport table Changed Files Updated : DbSchema NSKFDC-App.xlsx, masterSql.sql
</commit_message>
<xml_diff>
--- a/Database/DbSchema/DbSchema NSKFDC-App.xlsx
+++ b/Database/DbSchema/DbSchema NSKFDC-App.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mannu Kumari\Desktop\Assessment\trunk\Database\DbSchema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\NSKFDC-App\trunk\Database\DbSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1759494E-8278-4F2E-A52B-0549F74B81E0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t>Candidate</t>
   </si>
@@ -212,12 +213,6 @@
     <t>role</t>
   </si>
   <si>
-    <t xml:space="preserve"> trainingPartnerEmail - FK</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> trainingPartnerEmail - unique</t>
-  </si>
-  <si>
     <t>batchId-FK</t>
   </si>
   <si>
@@ -278,55 +273,31 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>trainingPartnerEmail - FK</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
     <t>GenerateReports</t>
   </si>
   <si>
-    <t>NSKFDCSheet - Flag</t>
-  </si>
-  <si>
-    <t>occupationReport - Flag</t>
-  </si>
-  <si>
-    <t>SDMSSheet - Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selectionCommittee - Flag </t>
-  </si>
-  <si>
-    <t>batchReport - Flag</t>
-  </si>
-  <si>
-    <t>ORGeneratedOn</t>
-  </si>
-  <si>
-    <t>ASGeneratedOn</t>
-  </si>
-  <si>
-    <t>NSKFDCGeneratedOn</t>
-  </si>
-  <si>
-    <t>SDMSGeneratedOn</t>
-  </si>
-  <si>
-    <t>SCGeneratedOn</t>
-  </si>
-  <si>
-    <t>BRGeneratedOn</t>
-  </si>
-  <si>
-    <t>generateReportsId (Auto Increment )- PK</t>
+    <t>generateReportsId - PK</t>
+  </si>
+  <si>
+    <t>reportType</t>
+  </si>
+  <si>
+    <t>generatedOn</t>
+  </si>
+  <si>
+    <t>userEmail</t>
+  </si>
+  <si>
+    <t>userEmail-FK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,8 +422,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +453,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -794,11 +765,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +803,7 @@
         <v>38</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -850,13 +821,13 @@
       <c r="G3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>97</v>
+      <c r="I3" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>62</v>
+      <c r="A4" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>1</v>
@@ -870,7 +841,7 @@
         <v>40</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -889,7 +860,7 @@
         <v>41</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -907,11 +878,14 @@
       <c r="G6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>73</v>
+      <c r="I6" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -920,10 +894,10 @@
         <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>82</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>92</v>
+        <v>80</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -934,13 +908,10 @@
       <c r="G8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>13</v>
@@ -950,15 +921,12 @@
         <v>30</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>14</v>
@@ -968,13 +936,10 @@
         <v>31</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="5" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>15</v>
@@ -984,15 +949,12 @@
         <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>16</v>
@@ -1004,19 +966,16 @@
       <c r="G12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>35</v>
@@ -1024,31 +983,25 @@
       <c r="G13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="16" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>6</v>
@@ -1060,16 +1013,13 @@
       <c r="G15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="5" t="s">
@@ -1078,13 +1028,10 @@
       <c r="G16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>7</v>
@@ -1094,15 +1041,12 @@
         <v>45</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
@@ -1112,9 +1056,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>9</v>
@@ -1124,9 +1068,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>10</v>
@@ -1139,24 +1083,24 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>19</v>
@@ -1166,9 +1110,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>20</v>
@@ -1178,9 +1122,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>21</v>
@@ -1190,35 +1134,35 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>